<commit_message>
Finalized Proto board with 3 way and 2 way switches included for on/off GSM and for on/off/test the board
</commit_message>
<xml_diff>
--- a/Teensy36_I2S_Proto/Teensy_Proto_BOM_Final.xlsx
+++ b/Teensy36_I2S_Proto/Teensy_Proto_BOM_Final.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68086EC-F18C-46EB-A659-B6CBF5747B6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D42D16-4668-4CCF-B5E8-0D327483FF96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Wildly_Proto_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="145">
   <si>
     <t>Wildly_Teensy_Proto_BOM</t>
   </si>
@@ -444,9 +444,6 @@
     <t>S1</t>
   </si>
   <si>
-    <t>Power</t>
-  </si>
-  <si>
     <t>Through Hole</t>
   </si>
   <si>
@@ -496,13 +493,34 @@
   </si>
   <si>
     <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.in/product-detail/en/c-k/OS103011MS8QP1/CKN9543-ND/1981414</t>
+  </si>
+  <si>
+    <t>OS103011MS8QP1</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE SP3T 100MA 12V</t>
+  </si>
+  <si>
+    <t>3 way slide switch</t>
+  </si>
+  <si>
+    <t>2 way slide switch</t>
+  </si>
+  <si>
+    <t>S2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,6 +567,24 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -599,7 +635,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -658,6 +694,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -939,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IS26"/>
+  <dimension ref="A1:IS27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3419,7 +3471,7 @@
       <c r="IR9" s="1"/>
       <c r="IS9" s="1"/>
     </row>
-    <row r="10" spans="1:253" s="2" customFormat="1" ht="25.5">
+    <row r="10" spans="1:253" s="2" customFormat="1">
       <c r="A10" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5065,7 +5117,7 @@
     </row>
     <row r="16" spans="1:253" s="2" customFormat="1" ht="30">
       <c r="A16" s="17">
-        <f t="shared" ref="A16:A26" si="1">ROW()-2</f>
+        <f t="shared" ref="A16:A27" si="1">ROW()-2</f>
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -7269,30 +7321,30 @@
     </row>
     <row r="24" spans="1:253" s="2" customFormat="1">
       <c r="A24" s="17">
-        <f t="shared" si="1"/>
+        <f>ROW()-2</f>
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>120</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="G24" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="H24" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="J24" s="6">
         <v>10</v>
@@ -7541,311 +7593,64 @@
       <c r="IR24" s="1"/>
       <c r="IS24" s="1"/>
     </row>
-    <row r="25" spans="1:253" s="2" customFormat="1" ht="30">
-      <c r="A25" s="17">
+    <row r="25" spans="1:253" s="25" customFormat="1">
+      <c r="A25" s="20">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="J25" s="7">
-        <v>10</v>
-      </c>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="1"/>
-      <c r="AC25" s="1"/>
-      <c r="AD25" s="1"/>
-      <c r="AE25" s="1"/>
-      <c r="AF25" s="1"/>
-      <c r="AG25" s="1"/>
-      <c r="AH25" s="1"/>
-      <c r="AI25" s="1"/>
-      <c r="AJ25" s="1"/>
-      <c r="AK25" s="1"/>
-      <c r="AL25" s="1"/>
-      <c r="AM25" s="1"/>
-      <c r="AN25" s="1"/>
-      <c r="AO25" s="1"/>
-      <c r="AP25" s="1"/>
-      <c r="AQ25" s="1"/>
-      <c r="AR25" s="1"/>
-      <c r="AS25" s="1"/>
-      <c r="AT25" s="1"/>
-      <c r="AU25" s="1"/>
-      <c r="AV25" s="1"/>
-      <c r="AW25" s="1"/>
-      <c r="AX25" s="1"/>
-      <c r="AY25" s="1"/>
-      <c r="AZ25" s="1"/>
-      <c r="BA25" s="1"/>
-      <c r="BB25" s="1"/>
-      <c r="BC25" s="1"/>
-      <c r="BD25" s="1"/>
-      <c r="BE25" s="1"/>
-      <c r="BF25" s="1"/>
-      <c r="BG25" s="1"/>
-      <c r="BH25" s="1"/>
-      <c r="BI25" s="1"/>
-      <c r="BJ25" s="1"/>
-      <c r="BK25" s="1"/>
-      <c r="BL25" s="1"/>
-      <c r="BM25" s="1"/>
-      <c r="BN25" s="1"/>
-      <c r="BO25" s="1"/>
-      <c r="BP25" s="1"/>
-      <c r="BQ25" s="1"/>
-      <c r="BR25" s="1"/>
-      <c r="BS25" s="1"/>
-      <c r="BT25" s="1"/>
-      <c r="BU25" s="1"/>
-      <c r="BV25" s="1"/>
-      <c r="BW25" s="1"/>
-      <c r="BX25" s="1"/>
-      <c r="BY25" s="1"/>
-      <c r="BZ25" s="1"/>
-      <c r="CA25" s="1"/>
-      <c r="CB25" s="1"/>
-      <c r="CC25" s="1"/>
-      <c r="CD25" s="1"/>
-      <c r="CE25" s="1"/>
-      <c r="CF25" s="1"/>
-      <c r="CG25" s="1"/>
-      <c r="CH25" s="1"/>
-      <c r="CI25" s="1"/>
-      <c r="CJ25" s="1"/>
-      <c r="CK25" s="1"/>
-      <c r="CL25" s="1"/>
-      <c r="CM25" s="1"/>
-      <c r="CN25" s="1"/>
-      <c r="CO25" s="1"/>
-      <c r="CP25" s="1"/>
-      <c r="CQ25" s="1"/>
-      <c r="CR25" s="1"/>
-      <c r="CS25" s="1"/>
-      <c r="CT25" s="1"/>
-      <c r="CU25" s="1"/>
-      <c r="CV25" s="1"/>
-      <c r="CW25" s="1"/>
-      <c r="CX25" s="1"/>
-      <c r="CY25" s="1"/>
-      <c r="CZ25" s="1"/>
-      <c r="DA25" s="1"/>
-      <c r="DB25" s="1"/>
-      <c r="DC25" s="1"/>
-      <c r="DD25" s="1"/>
-      <c r="DE25" s="1"/>
-      <c r="DF25" s="1"/>
-      <c r="DG25" s="1"/>
-      <c r="DH25" s="1"/>
-      <c r="DI25" s="1"/>
-      <c r="DJ25" s="1"/>
-      <c r="DK25" s="1"/>
-      <c r="DL25" s="1"/>
-      <c r="DM25" s="1"/>
-      <c r="DN25" s="1"/>
-      <c r="DO25" s="1"/>
-      <c r="DP25" s="1"/>
-      <c r="DQ25" s="1"/>
-      <c r="DR25" s="1"/>
-      <c r="DS25" s="1"/>
-      <c r="DT25" s="1"/>
-      <c r="DU25" s="1"/>
-      <c r="DV25" s="1"/>
-      <c r="DW25" s="1"/>
-      <c r="DX25" s="1"/>
-      <c r="DY25" s="1"/>
-      <c r="DZ25" s="1"/>
-      <c r="EA25" s="1"/>
-      <c r="EB25" s="1"/>
-      <c r="EC25" s="1"/>
-      <c r="ED25" s="1"/>
-      <c r="EE25" s="1"/>
-      <c r="EF25" s="1"/>
-      <c r="EG25" s="1"/>
-      <c r="EH25" s="1"/>
-      <c r="EI25" s="1"/>
-      <c r="EJ25" s="1"/>
-      <c r="EK25" s="1"/>
-      <c r="EL25" s="1"/>
-      <c r="EM25" s="1"/>
-      <c r="EN25" s="1"/>
-      <c r="EO25" s="1"/>
-      <c r="EP25" s="1"/>
-      <c r="EQ25" s="1"/>
-      <c r="ER25" s="1"/>
-      <c r="ES25" s="1"/>
-      <c r="ET25" s="1"/>
-      <c r="EU25" s="1"/>
-      <c r="EV25" s="1"/>
-      <c r="EW25" s="1"/>
-      <c r="EX25" s="1"/>
-      <c r="EY25" s="1"/>
-      <c r="EZ25" s="1"/>
-      <c r="FA25" s="1"/>
-      <c r="FB25" s="1"/>
-      <c r="FC25" s="1"/>
-      <c r="FD25" s="1"/>
-      <c r="FE25" s="1"/>
-      <c r="FF25" s="1"/>
-      <c r="FG25" s="1"/>
-      <c r="FH25" s="1"/>
-      <c r="FI25" s="1"/>
-      <c r="FJ25" s="1"/>
-      <c r="FK25" s="1"/>
-      <c r="FL25" s="1"/>
-      <c r="FM25" s="1"/>
-      <c r="FN25" s="1"/>
-      <c r="FO25" s="1"/>
-      <c r="FP25" s="1"/>
-      <c r="FQ25" s="1"/>
-      <c r="FR25" s="1"/>
-      <c r="FS25" s="1"/>
-      <c r="FT25" s="1"/>
-      <c r="FU25" s="1"/>
-      <c r="FV25" s="1"/>
-      <c r="FW25" s="1"/>
-      <c r="FX25" s="1"/>
-      <c r="FY25" s="1"/>
-      <c r="FZ25" s="1"/>
-      <c r="GA25" s="1"/>
-      <c r="GB25" s="1"/>
-      <c r="GC25" s="1"/>
-      <c r="GD25" s="1"/>
-      <c r="GE25" s="1"/>
-      <c r="GF25" s="1"/>
-      <c r="GG25" s="1"/>
-      <c r="GH25" s="1"/>
-      <c r="GI25" s="1"/>
-      <c r="GJ25" s="1"/>
-      <c r="GK25" s="1"/>
-      <c r="GL25" s="1"/>
-      <c r="GM25" s="1"/>
-      <c r="GN25" s="1"/>
-      <c r="GO25" s="1"/>
-      <c r="GP25" s="1"/>
-      <c r="GQ25" s="1"/>
-      <c r="GR25" s="1"/>
-      <c r="GS25" s="1"/>
-      <c r="GT25" s="1"/>
-      <c r="GU25" s="1"/>
-      <c r="GV25" s="1"/>
-      <c r="GW25" s="1"/>
-      <c r="GX25" s="1"/>
-      <c r="GY25" s="1"/>
-      <c r="GZ25" s="1"/>
-      <c r="HA25" s="1"/>
-      <c r="HB25" s="1"/>
-      <c r="HC25" s="1"/>
-      <c r="HD25" s="1"/>
-      <c r="HE25" s="1"/>
-      <c r="HF25" s="1"/>
-      <c r="HG25" s="1"/>
-      <c r="HH25" s="1"/>
-      <c r="HI25" s="1"/>
-      <c r="HJ25" s="1"/>
-      <c r="HK25" s="1"/>
-      <c r="HL25" s="1"/>
-      <c r="HM25" s="1"/>
-      <c r="HN25" s="1"/>
-      <c r="HO25" s="1"/>
-      <c r="HP25" s="1"/>
-      <c r="HQ25" s="1"/>
-      <c r="HR25" s="1"/>
-      <c r="HS25" s="1"/>
-      <c r="HT25" s="1"/>
-      <c r="HU25" s="1"/>
-      <c r="HV25" s="1"/>
-      <c r="HW25" s="1"/>
-      <c r="HX25" s="1"/>
-      <c r="HY25" s="1"/>
-      <c r="HZ25" s="1"/>
-      <c r="IA25" s="1"/>
-      <c r="IB25" s="1"/>
-      <c r="IC25" s="1"/>
-      <c r="ID25" s="1"/>
-      <c r="IE25" s="1"/>
-      <c r="IF25" s="1"/>
-      <c r="IG25" s="1"/>
-      <c r="IH25" s="1"/>
-      <c r="II25" s="1"/>
-      <c r="IJ25" s="1"/>
-      <c r="IK25" s="1"/>
-      <c r="IL25" s="1"/>
-      <c r="IM25" s="1"/>
-      <c r="IN25" s="1"/>
-      <c r="IO25" s="1"/>
-      <c r="IP25" s="1"/>
-      <c r="IQ25" s="1"/>
-      <c r="IR25" s="1"/>
-      <c r="IS25" s="1"/>
+      <c r="B25" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="23"/>
+      <c r="E25" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G25" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="J25" s="23"/>
     </row>
-    <row r="26" spans="1:253" s="2" customFormat="1">
+    <row r="26" spans="1:253" s="2" customFormat="1" ht="30">
       <c r="A26" s="17">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>134</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D26" s="6"/>
       <c r="E26" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>136</v>
+        <v>121</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="J26" s="7">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -8091,6 +7896,282 @@
       <c r="IR26" s="1"/>
       <c r="IS26" s="1"/>
     </row>
+    <row r="27" spans="1:253" s="2" customFormat="1">
+      <c r="A27" s="17">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="J27" s="7">
+        <v>25</v>
+      </c>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+      <c r="AI27" s="1"/>
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="1"/>
+      <c r="AL27" s="1"/>
+      <c r="AM27" s="1"/>
+      <c r="AN27" s="1"/>
+      <c r="AO27" s="1"/>
+      <c r="AP27" s="1"/>
+      <c r="AQ27" s="1"/>
+      <c r="AR27" s="1"/>
+      <c r="AS27" s="1"/>
+      <c r="AT27" s="1"/>
+      <c r="AU27" s="1"/>
+      <c r="AV27" s="1"/>
+      <c r="AW27" s="1"/>
+      <c r="AX27" s="1"/>
+      <c r="AY27" s="1"/>
+      <c r="AZ27" s="1"/>
+      <c r="BA27" s="1"/>
+      <c r="BB27" s="1"/>
+      <c r="BC27" s="1"/>
+      <c r="BD27" s="1"/>
+      <c r="BE27" s="1"/>
+      <c r="BF27" s="1"/>
+      <c r="BG27" s="1"/>
+      <c r="BH27" s="1"/>
+      <c r="BI27" s="1"/>
+      <c r="BJ27" s="1"/>
+      <c r="BK27" s="1"/>
+      <c r="BL27" s="1"/>
+      <c r="BM27" s="1"/>
+      <c r="BN27" s="1"/>
+      <c r="BO27" s="1"/>
+      <c r="BP27" s="1"/>
+      <c r="BQ27" s="1"/>
+      <c r="BR27" s="1"/>
+      <c r="BS27" s="1"/>
+      <c r="BT27" s="1"/>
+      <c r="BU27" s="1"/>
+      <c r="BV27" s="1"/>
+      <c r="BW27" s="1"/>
+      <c r="BX27" s="1"/>
+      <c r="BY27" s="1"/>
+      <c r="BZ27" s="1"/>
+      <c r="CA27" s="1"/>
+      <c r="CB27" s="1"/>
+      <c r="CC27" s="1"/>
+      <c r="CD27" s="1"/>
+      <c r="CE27" s="1"/>
+      <c r="CF27" s="1"/>
+      <c r="CG27" s="1"/>
+      <c r="CH27" s="1"/>
+      <c r="CI27" s="1"/>
+      <c r="CJ27" s="1"/>
+      <c r="CK27" s="1"/>
+      <c r="CL27" s="1"/>
+      <c r="CM27" s="1"/>
+      <c r="CN27" s="1"/>
+      <c r="CO27" s="1"/>
+      <c r="CP27" s="1"/>
+      <c r="CQ27" s="1"/>
+      <c r="CR27" s="1"/>
+      <c r="CS27" s="1"/>
+      <c r="CT27" s="1"/>
+      <c r="CU27" s="1"/>
+      <c r="CV27" s="1"/>
+      <c r="CW27" s="1"/>
+      <c r="CX27" s="1"/>
+      <c r="CY27" s="1"/>
+      <c r="CZ27" s="1"/>
+      <c r="DA27" s="1"/>
+      <c r="DB27" s="1"/>
+      <c r="DC27" s="1"/>
+      <c r="DD27" s="1"/>
+      <c r="DE27" s="1"/>
+      <c r="DF27" s="1"/>
+      <c r="DG27" s="1"/>
+      <c r="DH27" s="1"/>
+      <c r="DI27" s="1"/>
+      <c r="DJ27" s="1"/>
+      <c r="DK27" s="1"/>
+      <c r="DL27" s="1"/>
+      <c r="DM27" s="1"/>
+      <c r="DN27" s="1"/>
+      <c r="DO27" s="1"/>
+      <c r="DP27" s="1"/>
+      <c r="DQ27" s="1"/>
+      <c r="DR27" s="1"/>
+      <c r="DS27" s="1"/>
+      <c r="DT27" s="1"/>
+      <c r="DU27" s="1"/>
+      <c r="DV27" s="1"/>
+      <c r="DW27" s="1"/>
+      <c r="DX27" s="1"/>
+      <c r="DY27" s="1"/>
+      <c r="DZ27" s="1"/>
+      <c r="EA27" s="1"/>
+      <c r="EB27" s="1"/>
+      <c r="EC27" s="1"/>
+      <c r="ED27" s="1"/>
+      <c r="EE27" s="1"/>
+      <c r="EF27" s="1"/>
+      <c r="EG27" s="1"/>
+      <c r="EH27" s="1"/>
+      <c r="EI27" s="1"/>
+      <c r="EJ27" s="1"/>
+      <c r="EK27" s="1"/>
+      <c r="EL27" s="1"/>
+      <c r="EM27" s="1"/>
+      <c r="EN27" s="1"/>
+      <c r="EO27" s="1"/>
+      <c r="EP27" s="1"/>
+      <c r="EQ27" s="1"/>
+      <c r="ER27" s="1"/>
+      <c r="ES27" s="1"/>
+      <c r="ET27" s="1"/>
+      <c r="EU27" s="1"/>
+      <c r="EV27" s="1"/>
+      <c r="EW27" s="1"/>
+      <c r="EX27" s="1"/>
+      <c r="EY27" s="1"/>
+      <c r="EZ27" s="1"/>
+      <c r="FA27" s="1"/>
+      <c r="FB27" s="1"/>
+      <c r="FC27" s="1"/>
+      <c r="FD27" s="1"/>
+      <c r="FE27" s="1"/>
+      <c r="FF27" s="1"/>
+      <c r="FG27" s="1"/>
+      <c r="FH27" s="1"/>
+      <c r="FI27" s="1"/>
+      <c r="FJ27" s="1"/>
+      <c r="FK27" s="1"/>
+      <c r="FL27" s="1"/>
+      <c r="FM27" s="1"/>
+      <c r="FN27" s="1"/>
+      <c r="FO27" s="1"/>
+      <c r="FP27" s="1"/>
+      <c r="FQ27" s="1"/>
+      <c r="FR27" s="1"/>
+      <c r="FS27" s="1"/>
+      <c r="FT27" s="1"/>
+      <c r="FU27" s="1"/>
+      <c r="FV27" s="1"/>
+      <c r="FW27" s="1"/>
+      <c r="FX27" s="1"/>
+      <c r="FY27" s="1"/>
+      <c r="FZ27" s="1"/>
+      <c r="GA27" s="1"/>
+      <c r="GB27" s="1"/>
+      <c r="GC27" s="1"/>
+      <c r="GD27" s="1"/>
+      <c r="GE27" s="1"/>
+      <c r="GF27" s="1"/>
+      <c r="GG27" s="1"/>
+      <c r="GH27" s="1"/>
+      <c r="GI27" s="1"/>
+      <c r="GJ27" s="1"/>
+      <c r="GK27" s="1"/>
+      <c r="GL27" s="1"/>
+      <c r="GM27" s="1"/>
+      <c r="GN27" s="1"/>
+      <c r="GO27" s="1"/>
+      <c r="GP27" s="1"/>
+      <c r="GQ27" s="1"/>
+      <c r="GR27" s="1"/>
+      <c r="GS27" s="1"/>
+      <c r="GT27" s="1"/>
+      <c r="GU27" s="1"/>
+      <c r="GV27" s="1"/>
+      <c r="GW27" s="1"/>
+      <c r="GX27" s="1"/>
+      <c r="GY27" s="1"/>
+      <c r="GZ27" s="1"/>
+      <c r="HA27" s="1"/>
+      <c r="HB27" s="1"/>
+      <c r="HC27" s="1"/>
+      <c r="HD27" s="1"/>
+      <c r="HE27" s="1"/>
+      <c r="HF27" s="1"/>
+      <c r="HG27" s="1"/>
+      <c r="HH27" s="1"/>
+      <c r="HI27" s="1"/>
+      <c r="HJ27" s="1"/>
+      <c r="HK27" s="1"/>
+      <c r="HL27" s="1"/>
+      <c r="HM27" s="1"/>
+      <c r="HN27" s="1"/>
+      <c r="HO27" s="1"/>
+      <c r="HP27" s="1"/>
+      <c r="HQ27" s="1"/>
+      <c r="HR27" s="1"/>
+      <c r="HS27" s="1"/>
+      <c r="HT27" s="1"/>
+      <c r="HU27" s="1"/>
+      <c r="HV27" s="1"/>
+      <c r="HW27" s="1"/>
+      <c r="HX27" s="1"/>
+      <c r="HY27" s="1"/>
+      <c r="HZ27" s="1"/>
+      <c r="IA27" s="1"/>
+      <c r="IB27" s="1"/>
+      <c r="IC27" s="1"/>
+      <c r="ID27" s="1"/>
+      <c r="IE27" s="1"/>
+      <c r="IF27" s="1"/>
+      <c r="IG27" s="1"/>
+      <c r="IH27" s="1"/>
+      <c r="II27" s="1"/>
+      <c r="IJ27" s="1"/>
+      <c r="IK27" s="1"/>
+      <c r="IL27" s="1"/>
+      <c r="IM27" s="1"/>
+      <c r="IN27" s="1"/>
+      <c r="IO27" s="1"/>
+      <c r="IP27" s="1"/>
+      <c r="IQ27" s="1"/>
+      <c r="IR27" s="1"/>
+      <c r="IS27" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
@@ -8115,8 +8196,9 @@
     <hyperlink ref="G23" r:id="rId17" xr:uid="{5DEDF601-B897-43B6-8CB9-C1982589AF5C}"/>
     <hyperlink ref="G8" r:id="rId18" xr:uid="{B23123E4-5579-4F9D-A640-C750D942585D}"/>
     <hyperlink ref="G24" r:id="rId19" xr:uid="{D316D4B3-C9A3-40A1-BCE0-FD3D8F587200}"/>
-    <hyperlink ref="G25" r:id="rId20" xr:uid="{F2261AF0-A2FD-4A2C-9CA4-00CB8FB99173}"/>
-    <hyperlink ref="G26" r:id="rId21" xr:uid="{1F9D5E78-C47D-4874-A703-45254A4311B8}"/>
+    <hyperlink ref="G26" r:id="rId20" xr:uid="{F2261AF0-A2FD-4A2C-9CA4-00CB8FB99173}"/>
+    <hyperlink ref="G27" r:id="rId21" xr:uid="{1F9D5E78-C47D-4874-A703-45254A4311B8}"/>
+    <hyperlink ref="G25" r:id="rId22" xr:uid="{115E5BAC-35DE-4A68-8415-AAA828EF93FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>